<commit_message>
added solar charging with auto switching for AC supply charging. added POT for control
</commit_message>
<xml_diff>
--- a/ProjectOutputs/BOM/Bill of Materials-gorilla mist project.xlsx
+++ b/ProjectOutputs/BOM/Bill of Materials-gorilla mist project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="8895"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-gorilla mist " sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="164">
   <si>
     <t>Comment</t>
   </si>
@@ -39,13 +39,25 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Supplier 1</t>
+  </si>
+  <si>
+    <t>Supplier Unit Price 1</t>
+  </si>
+  <si>
     <t>T491D107K016AT</t>
   </si>
   <si>
     <t>Solid Tantalum Chip Capacitor, Standard T491 Series - Industrial Grade</t>
   </si>
   <si>
-    <t>C3, C6</t>
+    <t>C3, C6, C19</t>
   </si>
   <si>
     <t>D</t>
@@ -54,6 +66,9 @@
     <t>100uF</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>C0603C104K3RACTU</t>
   </si>
   <si>
@@ -72,7 +87,7 @@
     <t>T491A106K010AT</t>
   </si>
   <si>
-    <t>C7, C8, C12, C13</t>
+    <t>C7, C8, C12, C13, C21, C24</t>
   </si>
   <si>
     <t>A</t>
@@ -84,7 +99,7 @@
     <t>T491A225K010AT</t>
   </si>
   <si>
-    <t>C9</t>
+    <t>C9, C20</t>
   </si>
   <si>
     <t>2.2uF</t>
@@ -114,6 +129,18 @@
     <t>0.1uF</t>
   </si>
   <si>
+    <t>C0603C223K1RACTU</t>
+  </si>
+  <si>
+    <t>C22, C23</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
     <t>HSMB-C190</t>
   </si>
   <si>
@@ -126,9 +153,6 @@
     <t>1.6X0.8X0.8</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>SSC54</t>
   </si>
   <si>
@@ -171,7 +195,7 @@
     <t>Power Connector, Micro-Fit 3.0 Header, SMT, Single Row, Right Angle, 2 Circuits</t>
   </si>
   <si>
-    <t>J1, J2, J3, J4</t>
+    <t>J1, J2, J3, J4, J6, J7</t>
   </si>
   <si>
     <t>PJ-014DH-SMT</t>
@@ -183,7 +207,7 @@
     <t>J5</t>
   </si>
   <si>
-    <t>IHLP2525CZERxRxM11</t>
+    <t>IHLP2525CZER3R3M01</t>
   </si>
   <si>
     <t>Low Profile, High Current IHLP Inductor, 1uH to 22uH, 2.5 to 9A saturation current</t>
@@ -195,6 +219,18 @@
     <t>IHLP</t>
   </si>
   <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>IHLP2525CZER6R8M01</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
     <t>67996-406HLF</t>
   </si>
   <si>
@@ -240,7 +276,7 @@
     <t>HEXFET Power MOSFET</t>
   </si>
   <si>
-    <t>Q1</t>
+    <t>Q1, Q4</t>
   </si>
   <si>
     <t>TO-252AA_N</t>
@@ -252,13 +288,25 @@
     <t>Q2, Q3</t>
   </si>
   <si>
+    <t>IRLML6402TRPBF</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Micro3_N</t>
+  </si>
+  <si>
+    <t>International Rectifier</t>
+  </si>
+  <si>
     <t>ERJ3GEYJ101V</t>
   </si>
   <si>
     <t>Thick Film Chip Resistor, 1 Ohm to 10M Ohm Range, 5% Tolerance, 0603 Size, 0.1 W</t>
   </si>
   <si>
-    <t>R1, R14</t>
+    <t>R1, R14, R17</t>
   </si>
   <si>
     <t>3-0603</t>
@@ -342,13 +390,13 @@
     <t>100k</t>
   </si>
   <si>
-    <t>ERJ3EKF2212V</t>
+    <t>ERJ-3EKF1372V</t>
   </si>
   <si>
     <t>R12</t>
   </si>
   <si>
-    <t>22.1k</t>
+    <t>Panasonic Electronic Components</t>
   </si>
   <si>
     <t>ERJ3EKF9311V</t>
@@ -363,12 +411,18 @@
     <t>ERJ3GEYJ434V</t>
   </si>
   <si>
-    <t>R15</t>
+    <t>R15, R19</t>
   </si>
   <si>
     <t>430k</t>
   </si>
   <si>
+    <t>ERJ-3GEYJ185V</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
     <t>PVB4-EE</t>
   </si>
   <si>
@@ -402,6 +456,9 @@
     <t>TS3B_N</t>
   </si>
   <si>
+    <t>National Semiconductor</t>
+  </si>
+  <si>
     <t>BQ24600</t>
   </si>
   <si>
@@ -412,6 +469,36 @@
   </si>
   <si>
     <t>QFN16</t>
+  </si>
+  <si>
+    <t>LTC3129EUD-1</t>
+  </si>
+  <si>
+    <t>IC REG BUCK BST PROG 0.2A 16QFN</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Linear Technology</t>
+  </si>
+  <si>
+    <t>LTC3129EUD-1#PBF</t>
+  </si>
+  <si>
+    <t>LTC4412</t>
+  </si>
+  <si>
+    <t>IC OR CTRLR SRC SELECT TSOT23-6</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>TSOT23-6N</t>
+  </si>
+  <si>
+    <t>LTC4412ES6#TRMPBF</t>
   </si>
   <si>
     <t>CSTCE16M0V53</t>
@@ -773,16 +860,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="18" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="10" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,316 +893,480 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3">
         <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.41599999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E13" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>65</v>
@@ -1119,378 +1375,568 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E18" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E20" s="3">
         <v>2</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E21" s="3">
         <v>2</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="3">
-        <v>3</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="G25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="3">
         <v>2</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="F26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" s="3">
+      <c r="C32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="3">
         <v>2</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="3">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E32" s="3">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="3">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="F34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E34" s="3">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E35" s="3">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>134</v>
@@ -1499,11 +1945,201 @@
         <v>1</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>